<commit_message>
added global parameters support
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/modelo MM - TALCA 28.12_v4.xlsx
+++ b/Code/Limpio/Excels/modelo MM - TALCA 28.12_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\6020.Inecon_ModeloVanMedicion\6020.Inecon_ModeloVanMedicion\Code\Limpio\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AED8918-BA52-4CF2-83C2-D02ACCA6D990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220D60BB-CC67-4A86-9483-D8636CF625F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="10" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos_Tarifas" sheetId="13" r:id="rId1"/>
@@ -18,21 +18,22 @@
     <sheet name="FLUJO E1" sheetId="14" r:id="rId3"/>
     <sheet name="FLUJO E1 GRANDE" sheetId="15" r:id="rId4"/>
     <sheet name="PARAMETROS" sheetId="7" r:id="rId5"/>
-    <sheet name="PARAMETROS_NEO" sheetId="11" r:id="rId6"/>
-    <sheet name="DATOS" sheetId="8" r:id="rId7"/>
-    <sheet name="CAUDAL MODIFICADO" sheetId="4" r:id="rId8"/>
-    <sheet name="PORC CAUDAL PENDIENTE" sheetId="6" r:id="rId9"/>
-    <sheet name="EDAD" sheetId="2" r:id="rId10"/>
-    <sheet name="PROGRAMA AUTOCONTROL" sheetId="5" r:id="rId11"/>
-    <sheet name="CLASES" sheetId="3" r:id="rId12"/>
-    <sheet name="REFERENCIA CLASES DECAIMIENTO" sheetId="10" r:id="rId13"/>
-    <sheet name="CAUDAL ORIGINAL" sheetId="1" r:id="rId14"/>
+    <sheet name="PARAMETROS GLOBALES" sheetId="16" r:id="rId6"/>
+    <sheet name="PARAMETROS POR LOCALIDAD" sheetId="11" r:id="rId7"/>
+    <sheet name="DATOS" sheetId="8" r:id="rId8"/>
+    <sheet name="CAUDAL MODIFICADO" sheetId="4" r:id="rId9"/>
+    <sheet name="PORC CAUDAL PENDIENTE" sheetId="6" r:id="rId10"/>
+    <sheet name="EDAD" sheetId="2" r:id="rId11"/>
+    <sheet name="PROGRAMA AUTOCONTROL" sheetId="5" r:id="rId12"/>
+    <sheet name="CLASES" sheetId="3" r:id="rId13"/>
+    <sheet name="REFERENCIA CLASES DECAIMIENTO" sheetId="10" r:id="rId14"/>
+    <sheet name="CAUDAL ORIGINAL" sheetId="1" r:id="rId15"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">DATOS!$A$1:$G$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">DATOS!$A$1:$G$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -123,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="343">
   <si>
     <t>Intervalo (l/h)</t>
   </si>
@@ -1137,6 +1138,21 @@
   </si>
   <si>
     <t>YUNGAY</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Para cálculo de VAN</t>
+  </si>
+  <si>
+    <t>Impuesto</t>
+  </si>
+  <si>
+    <t>Para cálculo de impuesto</t>
   </si>
 </sst>
 </file>
@@ -1613,7 +1629,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="173" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1981,6 +1997,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -2542,7 +2559,7 @@
   <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3891,6 +3908,167 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DB1F8B-C405-4F58-8F6C-0C5484A61A58}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="11.44140625" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="33">
+        <v>0.22764462012548461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0.7723553798745153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="33">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="33">
+        <v>0.19296252036422679</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0.80703747963577332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="33">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="147" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="148" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="149">
+        <v>0.93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="147" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="148" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="149">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33893B52-C613-45F2-BCEC-C9588C1CFA20}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -4237,11 +4415,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF05CA6D-B359-469D-BCFA-0D1A2EFC1F75}">
   <dimension ref="A1:F170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F56" sqref="F56:F170"/>
     </sheetView>
   </sheetViews>
@@ -6900,7 +7078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F81CE5B9-9D9E-4972-953E-3F823FF745DF}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -7023,7 +7201,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACB5FF1-7A28-46AB-AC06-FB476C488476}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -7099,7 +7277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9D5E7F-12B8-4A53-9E8A-63ABDC168AAE}">
   <dimension ref="A1:E37"/>
   <sheetViews>
@@ -24551,6 +24729,57 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19A73C1-5AB0-483A-B923-13CF32B17E6E}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="134" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" s="134" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="134" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="163">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="163">
+        <v>0.27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB82D1B7-7706-48C2-8EA7-60D7CFF145FF}">
   <dimension ref="A1:N6"/>
   <sheetViews>
@@ -24824,7 +25053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F3A346-95CC-40C7-A048-A8DCA15A773E}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -25460,7 +25689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3D49A9-06A7-46DC-9EBC-1914E499D5E6}">
   <dimension ref="A1:E37"/>
   <sheetViews>
@@ -26086,168 +26315,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5DB1F8B-C405-4F58-8F6C-0C5484A61A58}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="11.44140625" style="32"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="33">
-        <v>0.22764462012548461</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="33">
-        <v>0.7723553798745153</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="33">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="33">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="33">
-        <v>0.19296252036422679</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="33">
-        <v>0.80703747963577332</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="33">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="33">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="33">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="33">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="147" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="148" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="149">
-        <v>0.93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="147" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="148" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="149">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A39F2B8F08F82E47A51B7B9E2BB752C4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="9e705a7ec9ec7901fcdc888e6563d1f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="afef9374-bd24-49fe-b5be-cd056ccbd7a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ae930c13f3dbc9432d329521bd2e19c" ns3:_="">
     <xsd:import namespace="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
@@ -26435,24 +26520,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1944A5F0-70A3-4C8E-90B4-7B1083CA7BF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26468,28 +26560,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Funciona los VAN a menos de 2% de error
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/modelo MM - TALCA 28.12_v4.xlsx
+++ b/Code/Limpio/Excels/modelo MM - TALCA 28.12_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\6020.Inecon_ModeloVanMedicion\6020.Inecon_ModeloVanMedicion\Code\Limpio\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220D60BB-CC67-4A86-9483-D8636CF625F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF935BC-6E7E-4188-B751-59C2DBC44E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="5" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="5" activeTab="5" xr2:uid="{0B67A8E0-BE2B-4F48-8F89-95A6B35879D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos_Tarifas" sheetId="13" r:id="rId1"/>
@@ -1988,6 +1988,7 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1997,7 +1998,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -11006,7 +11006,7 @@
       <c r="V98" s="82"/>
     </row>
     <row r="99" spans="1:22" s="83" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="160" t="s">
+      <c r="B99" s="161" t="s">
         <v>167</v>
       </c>
       <c r="C99" s="84" t="s">
@@ -11033,7 +11033,7 @@
       <c r="S99" s="85"/>
     </row>
     <row r="100" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B100" s="161"/>
+      <c r="B100" s="162"/>
       <c r="C100" s="86"/>
       <c r="D100" s="87"/>
       <c r="E100" s="87"/>
@@ -11053,7 +11053,7 @@
       <c r="S100" s="87"/>
     </row>
     <row r="101" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="161"/>
+      <c r="B101" s="162"/>
       <c r="C101" s="83" t="s">
         <v>169</v>
       </c>
@@ -11078,7 +11078,7 @@
       <c r="S101" s="87"/>
     </row>
     <row r="102" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="161"/>
+      <c r="B102" s="162"/>
       <c r="D102" s="88"/>
       <c r="E102" s="88"/>
       <c r="F102" s="88"/>
@@ -11097,7 +11097,7 @@
       <c r="S102" s="88"/>
     </row>
     <row r="103" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="161"/>
+      <c r="B103" s="162"/>
       <c r="D103" s="88"/>
       <c r="E103" s="88"/>
       <c r="F103" s="88"/>
@@ -11116,7 +11116,7 @@
       <c r="S103" s="88"/>
     </row>
     <row r="104" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="161"/>
+      <c r="B104" s="162"/>
       <c r="C104" s="86" t="s">
         <v>170</v>
       </c>
@@ -11187,7 +11187,7 @@
       <c r="A105" s="83">
         <v>1</v>
       </c>
-      <c r="B105" s="161"/>
+      <c r="B105" s="162"/>
       <c r="C105" s="83" t="s">
         <v>171</v>
       </c>
@@ -11255,7 +11255,7 @@
       <c r="U105" s="89"/>
     </row>
     <row r="106" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B106" s="161"/>
+      <c r="B106" s="162"/>
       <c r="C106" s="90"/>
       <c r="D106" s="91"/>
       <c r="E106" s="92"/>
@@ -11275,7 +11275,7 @@
       <c r="S106" s="92"/>
     </row>
     <row r="107" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="161"/>
+      <c r="B107" s="162"/>
       <c r="C107" s="83" t="s">
         <v>172</v>
       </c>
@@ -11297,7 +11297,7 @@
       <c r="S107" s="88"/>
     </row>
     <row r="108" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="161"/>
+      <c r="B108" s="162"/>
       <c r="C108" s="93" t="s">
         <v>173</v>
       </c>
@@ -11323,7 +11323,7 @@
       <c r="T108" s="94"/>
     </row>
     <row r="109" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="161"/>
+      <c r="B109" s="162"/>
       <c r="C109" s="93" t="s">
         <v>174</v>
       </c>
@@ -11394,7 +11394,7 @@
       <c r="A110" s="83">
         <v>10</v>
       </c>
-      <c r="B110" s="161"/>
+      <c r="B110" s="162"/>
       <c r="C110" s="93" t="s">
         <v>175</v>
       </c>
@@ -11464,7 +11464,7 @@
       <c r="A111" s="95">
         <v>0.27</v>
       </c>
-      <c r="B111" s="162"/>
+      <c r="B111" s="163"/>
       <c r="C111" s="96" t="s">
         <v>176</v>
       </c>
@@ -17450,7 +17450,7 @@
       <c r="V99" s="82"/>
     </row>
     <row r="100" spans="1:22" s="83" customFormat="1" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="160" t="s">
+      <c r="B100" s="161" t="s">
         <v>167</v>
       </c>
       <c r="C100" s="84" t="s">
@@ -17477,7 +17477,7 @@
       <c r="S100" s="85"/>
     </row>
     <row r="101" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B101" s="161"/>
+      <c r="B101" s="162"/>
       <c r="C101" s="86"/>
       <c r="D101" s="87"/>
       <c r="E101" s="87"/>
@@ -17497,7 +17497,7 @@
       <c r="S101" s="87"/>
     </row>
     <row r="102" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B102" s="161"/>
+      <c r="B102" s="162"/>
       <c r="C102" s="83" t="s">
         <v>169</v>
       </c>
@@ -17522,7 +17522,7 @@
       <c r="S102" s="87"/>
     </row>
     <row r="103" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B103" s="161"/>
+      <c r="B103" s="162"/>
       <c r="D103" s="88"/>
       <c r="E103" s="88"/>
       <c r="F103" s="88"/>
@@ -17541,7 +17541,7 @@
       <c r="S103" s="88"/>
     </row>
     <row r="104" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B104" s="161"/>
+      <c r="B104" s="162"/>
       <c r="D104" s="88"/>
       <c r="E104" s="88"/>
       <c r="F104" s="88"/>
@@ -17560,7 +17560,7 @@
       <c r="S104" s="88"/>
     </row>
     <row r="105" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B105" s="161"/>
+      <c r="B105" s="162"/>
       <c r="C105" s="86" t="s">
         <v>170</v>
       </c>
@@ -17631,7 +17631,7 @@
       <c r="A106" s="83">
         <v>1</v>
       </c>
-      <c r="B106" s="161"/>
+      <c r="B106" s="162"/>
       <c r="C106" s="83" t="s">
         <v>171</v>
       </c>
@@ -17699,7 +17699,7 @@
       <c r="U106" s="89"/>
     </row>
     <row r="107" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B107" s="161"/>
+      <c r="B107" s="162"/>
       <c r="C107" s="90"/>
       <c r="D107" s="91"/>
       <c r="E107" s="92"/>
@@ -17719,7 +17719,7 @@
       <c r="S107" s="92"/>
     </row>
     <row r="108" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B108" s="161"/>
+      <c r="B108" s="162"/>
       <c r="C108" s="83" t="s">
         <v>172</v>
       </c>
@@ -17741,7 +17741,7 @@
       <c r="S108" s="88"/>
     </row>
     <row r="109" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="161"/>
+      <c r="B109" s="162"/>
       <c r="C109" s="93" t="s">
         <v>173</v>
       </c>
@@ -17767,7 +17767,7 @@
       <c r="T109" s="94"/>
     </row>
     <row r="110" spans="1:22" s="83" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="B110" s="161"/>
+      <c r="B110" s="162"/>
       <c r="C110" s="93" t="s">
         <v>174</v>
       </c>
@@ -17838,7 +17838,7 @@
       <c r="A111" s="83">
         <v>10</v>
       </c>
-      <c r="B111" s="161"/>
+      <c r="B111" s="162"/>
       <c r="C111" s="93" t="s">
         <v>175</v>
       </c>
@@ -17908,7 +17908,7 @@
       <c r="A112" s="95">
         <v>0.27</v>
       </c>
-      <c r="B112" s="162"/>
+      <c r="B112" s="163"/>
       <c r="C112" s="96" t="s">
         <v>176</v>
       </c>
@@ -21734,7 +21734,7 @@
       <c r="V50" s="82"/>
     </row>
     <row r="51" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="160" t="s">
+      <c r="B51" s="161" t="s">
         <v>167</v>
       </c>
       <c r="C51" s="84" t="s">
@@ -21792,7 +21792,7 @@
       </c>
     </row>
     <row r="52" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="161"/>
+      <c r="B52" s="162"/>
       <c r="C52" s="86"/>
       <c r="D52" s="87"/>
       <c r="E52" s="87"/>
@@ -21812,7 +21812,7 @@
       <c r="S52" s="87"/>
     </row>
     <row r="53" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="161"/>
+      <c r="B53" s="162"/>
       <c r="C53" s="83" t="s">
         <v>169</v>
       </c>
@@ -21834,7 +21834,7 @@
       <c r="S53" s="87"/>
     </row>
     <row r="54" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="161"/>
+      <c r="B54" s="162"/>
       <c r="D54" s="88"/>
       <c r="E54" s="88"/>
       <c r="F54" s="88"/>
@@ -21853,7 +21853,7 @@
       <c r="S54" s="88"/>
     </row>
     <row r="55" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="161"/>
+      <c r="B55" s="162"/>
       <c r="D55" s="88"/>
       <c r="E55" s="88"/>
       <c r="F55" s="88"/>
@@ -21872,7 +21872,7 @@
       <c r="S55" s="88"/>
     </row>
     <row r="56" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="161"/>
+      <c r="B56" s="162"/>
       <c r="C56" s="86" t="s">
         <v>170</v>
       </c>
@@ -21942,7 +21942,7 @@
       <c r="A57" s="83">
         <v>1</v>
       </c>
-      <c r="B57" s="161"/>
+      <c r="B57" s="162"/>
       <c r="C57" s="83" t="s">
         <v>171</v>
       </c>
@@ -22009,7 +22009,7 @@
       </c>
     </row>
     <row r="58" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="161"/>
+      <c r="B58" s="162"/>
       <c r="C58" s="90"/>
       <c r="D58" s="91"/>
       <c r="E58" s="92"/>
@@ -22029,7 +22029,7 @@
       <c r="S58" s="92"/>
     </row>
     <row r="59" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="161"/>
+      <c r="B59" s="162"/>
       <c r="C59" s="83" t="s">
         <v>172</v>
       </c>
@@ -22051,7 +22051,7 @@
       <c r="S59" s="88"/>
     </row>
     <row r="60" spans="1:22" s="83" customFormat="1" ht="13.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="161"/>
+      <c r="B60" s="162"/>
       <c r="C60" s="93" t="s">
         <v>173</v>
       </c>
@@ -22079,7 +22079,7 @@
       <c r="A61" s="83">
         <v>10</v>
       </c>
-      <c r="B61" s="161"/>
+      <c r="B61" s="162"/>
       <c r="C61" s="93" t="s">
         <v>175</v>
       </c>
@@ -22149,7 +22149,7 @@
       <c r="A62" s="95">
         <v>0.27</v>
       </c>
-      <c r="B62" s="162"/>
+      <c r="B62" s="163"/>
       <c r="C62" s="96" t="s">
         <v>176</v>
       </c>
@@ -24732,9 +24732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C19A73C1-5AB0-483A-B923-13CF32B17E6E}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -24756,7 +24754,7 @@
       <c r="A2" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="163">
+      <c r="B2" s="160">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C2" t="s">
@@ -24767,7 +24765,7 @@
       <c r="A3" t="s">
         <v>341</v>
       </c>
-      <c r="B3" s="163">
+      <c r="B3" s="160">
         <v>0.27</v>
       </c>
       <c r="C3" t="s">
@@ -26316,23 +26314,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A39F2B8F08F82E47A51B7B9E2BB752C4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="9e705a7ec9ec7901fcdc888e6563d1f3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="afef9374-bd24-49fe-b5be-cd056ccbd7a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ae930c13f3dbc9432d329521bd2e19c" ns3:_="">
     <xsd:import namespace="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
@@ -26520,31 +26501,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="afef9374-bd24-49fe-b5be-cd056ccbd7a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1944A5F0-70A3-4C8E-90B4-7B1083CA7BF2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26560,4 +26534,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{799D9F8D-2034-4116-9680-A411761E28F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F368767-011F-4603-B6D3-67B09FEB0E3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="afef9374-bd24-49fe-b5be-cd056ccbd7a9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>